<commit_message>
# Stable V1: `wafer_map_excel_ver2`
</commit_message>
<xml_diff>
--- a/pattern.xlsx
+++ b/pattern.xlsx
@@ -127,21 +127,6 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Chart with patterns</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
     <plotArea>
       <scatterChart>
         <ser>

</xml_diff>